<commit_message>
Complete rewrite of the internal logic
</commit_message>
<xml_diff>
--- a/XScouting/Scout/results.xlsx
+++ b/XScouting/Scout/results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Team Number</t>
   </si>
@@ -128,13 +128,16 @@
     <t>Middletown CT</t>
   </si>
   <si>
-    <t>Red</t>
+    <t>Blue</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t/>
+    <t>Tried but Failed</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
   <si>
     <t>No</t>
@@ -213,10 +216,10 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -372,8 +375,8 @@
       <c r="H3" t="n">
         <v>2.0</v>
       </c>
-      <c r="I3" t="s">
-        <v>39</v>
+      <c r="I3" t="n">
+        <v>2.0</v>
       </c>
       <c r="J3" t="n">
         <v>1.0</v>
@@ -402,8 +405,8 @@
       <c r="R3" t="n">
         <v>3.0</v>
       </c>
-      <c r="S3" t="n">
-        <v>2.0</v>
+      <c r="S3" t="s">
+        <v>40</v>
       </c>
       <c r="T3" t="n">
         <v>1.0</v>
@@ -433,16 +436,16 @@
         <v>2.0</v>
       </c>
       <c r="AC3" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="AD3" t="n">
-        <v>164.0</v>
+        <v>0.0</v>
       </c>
       <c r="AE3" t="n">
-        <v>7.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF3" t="n" s="3">
-        <v>187.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -470,8 +473,8 @@
       <c r="H4" t="n">
         <v>2.0</v>
       </c>
-      <c r="I4" t="s">
-        <v>39</v>
+      <c r="I4" t="n">
+        <v>2.0</v>
       </c>
       <c r="J4" t="n">
         <v>1.0</v>
@@ -500,8 +503,8 @@
       <c r="R4" t="n">
         <v>3.0</v>
       </c>
-      <c r="S4" t="n">
-        <v>2.0</v>
+      <c r="S4" t="s">
+        <v>40</v>
       </c>
       <c r="T4" t="n">
         <v>1.0</v>
@@ -531,16 +534,16 @@
         <v>2.0</v>
       </c>
       <c r="AC4" t="n">
-        <v>16.0</v>
+        <v>0.0</v>
       </c>
       <c r="AD4" t="n">
-        <v>164.0</v>
+        <v>0.0</v>
       </c>
       <c r="AE4" t="n">
-        <v>7.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF4" t="n" s="3">
-        <v>187.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -548,10 +551,10 @@
         <v>0.0</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
@@ -563,13 +566,13 @@
         <v>0.0</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
       </c>
-      <c r="I5" t="s">
-        <v>41</v>
+      <c r="I5" t="n">
+        <v>0.0</v>
       </c>
       <c r="J5" t="n">
         <v>0.0</v>
@@ -605,7 +608,7 @@
         <v>0.0</v>
       </c>
       <c r="U5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V5" t="n">
         <v>0.0</v>
@@ -635,16 +638,16 @@
         <v>0.0</v>
       </c>
       <c r="AE5" t="n">
-        <v>7.5</v>
+        <v>0.0</v>
       </c>
       <c r="AF5" t="n" s="3">
-        <v>7.5</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:K1"/>
     <mergeCell ref="L1:W1"/>
     <mergeCell ref="X1:AB1"/>
     <mergeCell ref="AC1:AF1"/>

</xml_diff>